<commit_message>
added feature for adding non ingredients to shopping list and updated shopping list
</commit_message>
<xml_diff>
--- a/data/additional_items.xlsx
+++ b/data/additional_items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\meal-plan\meal-plan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CAAC7C-A167-4671-B966-C91101D984FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9847CC9-4836-461B-8C44-1AF2C723C94B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="-2598" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>item</t>
   </si>
@@ -40,6 +40,18 @@
   </si>
   <si>
     <t>1 package of sliced turkey</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>non-ingredient</t>
+  </si>
+  <si>
+    <t>paper towels</t>
+  </si>
+  <si>
+    <t>toilet paper</t>
   </si>
 </sst>
 </file>
@@ -357,40 +369,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="55.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>